<commit_message>
tien long + vietglobal
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang6/1.NhanBH/NBH220629_MinhHuy.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang6/1.NhanBH/NBH220629_MinhHuy.xlsx
@@ -485,6 +485,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -523,45 +562,6 @@
     </xf>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,7 +919,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:F7"/>
+      <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -936,92 +936,92 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="6"/>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="49"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="28"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="35"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="48"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="51"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="44"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="46"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
@@ -1124,26 +1124,26 @@
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="42" t="s">
+      <c r="A16" s="50"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
     </row>
     <row r="17" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="26" t="s">
+      <c r="C17" s="49"/>
+      <c r="D17" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="40"/>
     </row>
     <row r="18" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
@@ -1179,16 +1179,16 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28" t="s">
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="42"/>
     </row>
     <row r="23" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
@@ -1216,13 +1216,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="B7:F7"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="B8:F8"/>
@@ -1231,6 +1224,13 @@
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>